<commit_message>
replace the gem "csv_hasher" with "csv" and make necessary related changes to the implementation.
</commit_message>
<xml_diff>
--- a/lib/btap/measures/UtilityTariffs/resources/utility_electricity_tariffs.xlsx
+++ b/lib/btap/measures/UtilityTariffs/resources/utility_electricity_tariffs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="27795" windowHeight="12840"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,21 +27,6 @@
     <t>Province</t>
   </si>
   <si>
-    <t>Monthly Charge ($)</t>
-  </si>
-  <si>
-    <t>Energy Charges Block 1 Limit (kWh)</t>
-  </si>
-  <si>
-    <t>Energy Charges Block 2 Limit (kWh)</t>
-  </si>
-  <si>
-    <t>Energy Charges Block 3 Limit (kWh)</t>
-  </si>
-  <si>
-    <t>Energy Charges Block 4 Limit (kWh)</t>
-  </si>
-  <si>
     <t>Montreal</t>
   </si>
   <si>
@@ -51,46 +36,61 @@
     <t>HydroQuebec</t>
   </si>
   <si>
-    <t>Energy Charges Block 2 Rate ($)</t>
-  </si>
-  <si>
-    <t>Energy Charges Block 1 Rate ($)</t>
-  </si>
-  <si>
-    <t>Energy Charges Block 3 Rate ($)</t>
-  </si>
-  <si>
-    <t>Energy Charges Block 4 Rate ($)</t>
-  </si>
-  <si>
-    <t>Energy Charges Block 5 Rate ($)</t>
-  </si>
-  <si>
-    <t>Demand Charges Block 1 Limit (kW)</t>
-  </si>
-  <si>
-    <t>Demand Charges Block 1 Rate ($)</t>
-  </si>
-  <si>
-    <t>Demand Charges Block 2 Limit (kW)</t>
-  </si>
-  <si>
-    <t>Demand Charges Block 2 Rate ($)</t>
-  </si>
-  <si>
-    <t>Demand Charges Block 3 Limit (kW)</t>
-  </si>
-  <si>
-    <t>Demand Charges Block 3 Rate ($)</t>
-  </si>
-  <si>
-    <t>Demand Charges Block 4 Limit (kW)</t>
-  </si>
-  <si>
-    <t>Demand Charges Block 4 Rate ($)</t>
-  </si>
-  <si>
-    <t>Demand Charges Block 5 Rate ($)</t>
+    <t>Energy_Charges_Block_1_Limit_(kWh)</t>
+  </si>
+  <si>
+    <t>Energy_Charges_Block_1_Rate_($)</t>
+  </si>
+  <si>
+    <t>Energy_Charges_Block_2_Limit_(kWh)</t>
+  </si>
+  <si>
+    <t>Energy_Charges_Block_2_Rate_($)</t>
+  </si>
+  <si>
+    <t>Energy_Charges_Block_3_Limit_(kWh)</t>
+  </si>
+  <si>
+    <t>Energy_Charges_Block_3_Rate_($)</t>
+  </si>
+  <si>
+    <t>Energy_Charges_Block_4_Limit_(kWh)</t>
+  </si>
+  <si>
+    <t>Energy_Charges_Block_4_Rate_($)</t>
+  </si>
+  <si>
+    <t>Energy_Charges_Block_5_Rate_($)</t>
+  </si>
+  <si>
+    <t>Demand_Charges_Block_1_Limit_(kW)</t>
+  </si>
+  <si>
+    <t>Demand_Charges_Block_1_Rate_($)</t>
+  </si>
+  <si>
+    <t>Demand_Charges_Block_2_Limit_(kW)</t>
+  </si>
+  <si>
+    <t>Demand_Charges_Block_2_Rate_($)</t>
+  </si>
+  <si>
+    <t>Demand_Charges_Block_3_Limit_(kW)</t>
+  </si>
+  <si>
+    <t>Demand_Charges_Block_3_Rate_($)</t>
+  </si>
+  <si>
+    <t>Demand_Charges_Block_4_Limit_(kW)</t>
+  </si>
+  <si>
+    <t>Demand_Charges_Block_4_Rate_($)</t>
+  </si>
+  <si>
+    <t>Demand_Charges_Block_5_Rate_($)</t>
+  </si>
+  <si>
+    <t>Monthly_Charge_($)</t>
   </si>
 </sst>
 </file>
@@ -432,7 +432,7 @@
   <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,72 +448,72 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>14</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>15</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>16</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>17</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>19</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>20</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>21</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>22</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>23</v>
-      </c>
-      <c r="V1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D2">
         <v>12.33</v>

</xml_diff>

<commit_message>
Use the city name in the location tag of the weather file to choose the tariff from the csv file. This approach has limitations when there is more than one tariff for the same city in the database. In this case the first tariff listed in the database for the city will be selected.
</commit_message>
<xml_diff>
--- a/lib/btap/measures/UtilityTariffs/resources/utility_electricity_tariffs.xlsx
+++ b/lib/btap/measures/UtilityTariffs/resources/utility_electricity_tariffs.xlsx
@@ -27,70 +27,70 @@
     <t>Province</t>
   </si>
   <si>
+    <t>Quebec</t>
+  </si>
+  <si>
+    <t>HydroQuebec</t>
+  </si>
+  <si>
+    <t>Energy_Charges_Block_1_Limit_(kWh)</t>
+  </si>
+  <si>
+    <t>Energy_Charges_Block_1_Rate_($)</t>
+  </si>
+  <si>
+    <t>Energy_Charges_Block_2_Limit_(kWh)</t>
+  </si>
+  <si>
+    <t>Energy_Charges_Block_2_Rate_($)</t>
+  </si>
+  <si>
+    <t>Energy_Charges_Block_3_Limit_(kWh)</t>
+  </si>
+  <si>
+    <t>Energy_Charges_Block_3_Rate_($)</t>
+  </si>
+  <si>
+    <t>Energy_Charges_Block_4_Limit_(kWh)</t>
+  </si>
+  <si>
+    <t>Energy_Charges_Block_4_Rate_($)</t>
+  </si>
+  <si>
+    <t>Energy_Charges_Block_5_Rate_($)</t>
+  </si>
+  <si>
+    <t>Demand_Charges_Block_1_Limit_(kW)</t>
+  </si>
+  <si>
+    <t>Demand_Charges_Block_1_Rate_($)</t>
+  </si>
+  <si>
+    <t>Demand_Charges_Block_2_Limit_(kW)</t>
+  </si>
+  <si>
+    <t>Demand_Charges_Block_2_Rate_($)</t>
+  </si>
+  <si>
+    <t>Demand_Charges_Block_3_Limit_(kW)</t>
+  </si>
+  <si>
+    <t>Demand_Charges_Block_3_Rate_($)</t>
+  </si>
+  <si>
+    <t>Demand_Charges_Block_4_Limit_(kW)</t>
+  </si>
+  <si>
+    <t>Demand_Charges_Block_4_Rate_($)</t>
+  </si>
+  <si>
+    <t>Demand_Charges_Block_5_Rate_($)</t>
+  </si>
+  <si>
+    <t>Monthly_Charge_($)</t>
+  </si>
+  <si>
     <t>Montreal</t>
-  </si>
-  <si>
-    <t>Quebec</t>
-  </si>
-  <si>
-    <t>HydroQuebec</t>
-  </si>
-  <si>
-    <t>Energy_Charges_Block_1_Limit_(kWh)</t>
-  </si>
-  <si>
-    <t>Energy_Charges_Block_1_Rate_($)</t>
-  </si>
-  <si>
-    <t>Energy_Charges_Block_2_Limit_(kWh)</t>
-  </si>
-  <si>
-    <t>Energy_Charges_Block_2_Rate_($)</t>
-  </si>
-  <si>
-    <t>Energy_Charges_Block_3_Limit_(kWh)</t>
-  </si>
-  <si>
-    <t>Energy_Charges_Block_3_Rate_($)</t>
-  </si>
-  <si>
-    <t>Energy_Charges_Block_4_Limit_(kWh)</t>
-  </si>
-  <si>
-    <t>Energy_Charges_Block_4_Rate_($)</t>
-  </si>
-  <si>
-    <t>Energy_Charges_Block_5_Rate_($)</t>
-  </si>
-  <si>
-    <t>Demand_Charges_Block_1_Limit_(kW)</t>
-  </si>
-  <si>
-    <t>Demand_Charges_Block_1_Rate_($)</t>
-  </si>
-  <si>
-    <t>Demand_Charges_Block_2_Limit_(kW)</t>
-  </si>
-  <si>
-    <t>Demand_Charges_Block_2_Rate_($)</t>
-  </si>
-  <si>
-    <t>Demand_Charges_Block_3_Limit_(kW)</t>
-  </si>
-  <si>
-    <t>Demand_Charges_Block_3_Rate_($)</t>
-  </si>
-  <si>
-    <t>Demand_Charges_Block_4_Limit_(kW)</t>
-  </si>
-  <si>
-    <t>Demand_Charges_Block_4_Rate_($)</t>
-  </si>
-  <si>
-    <t>Demand_Charges_Block_5_Rate_($)</t>
-  </si>
-  <si>
-    <t>Monthly_Charge_($)</t>
   </si>
 </sst>
 </file>
@@ -432,7 +432,7 @@
   <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,72 +448,72 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>13</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>14</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>15</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>16</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>18</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>19</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>20</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>21</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>22</v>
-      </c>
-      <c r="V1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
       </c>
       <c r="D2">
         <v>12.33</v>

</xml_diff>